<commit_message>
Ajout Borderpane et menuBar
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Antoine/Journal_Travail.xlsx
+++ b/Dossiers personnels/Antoine/Journal_Travail.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4C2FF2-564B-4D7B-AB6C-6647893E4E29}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +53,18 @@
   </si>
   <si>
     <t>Antoine Rochat</t>
+  </si>
+  <si>
+    <t>Discussion planification et organisation de groupe</t>
+  </si>
+  <si>
+    <t>Lecture du tutoriel JavaFX sur openclassroom</t>
+  </si>
+  <si>
+    <t>Visionnage de vidéos sur JavaFX et FXML sur la chaîne youtube thenewboston</t>
+  </si>
+  <si>
+    <t>Création du projet à l'aide d'une borderPane ainsi que création de la MenuBar</t>
   </si>
 </sst>
 </file>
@@ -452,7 +465,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -541,24 +554,48 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
+      <c r="A10" s="3">
+        <v>43166</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
+        <v>43169</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="3">
+        <v>43173</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="3">
+        <v>43175</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
@@ -656,7 +693,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>10.5</v>
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>